<commit_message>
re-org patternGen project code
</commit_message>
<xml_diff>
--- a/patternGen/PROTO1.xlsx
+++ b/patternGen/PROTO1.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Qihong/Dropbox/github/categorization_PDP/patternGen/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15900" tabRatio="500"/>
+    <workbookView xWindow="27080" yWindow="3720" windowWidth="25040" windowHeight="15900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,6 +98,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -421,12 +431,12 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>4</v>
       </c>
@@ -446,7 +456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -484,7 +494,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -522,7 +532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -560,7 +570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -598,7 +608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -639,10 +649,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>